<commit_message>
mongo lab creds updated
</commit_message>
<xml_diff>
--- a/Mongo-Creds.xlsx
+++ b/Mongo-Creds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ameen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Training\ANZ\Batch2\rresources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5363F1D-D29A-4181-9330-46819897E161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0E06B8-9756-461E-A73B-835B26012336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="7575" windowWidth="29040" windowHeight="15720" xr2:uid="{F8BF5C9E-07CF-441C-8345-B3004B2C3748}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" xr2:uid="{F8BF5C9E-07CF-441C-8345-B3004B2C3748}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>MongoDB-Training-986-1</t>
   </si>
@@ -197,12 +197,90 @@
       <t>https://trainee.cloudadda.com</t>
     </r>
   </si>
+  <si>
+    <t>Participant Name</t>
+  </si>
+  <si>
+    <t>Ashok Kumar</t>
+  </si>
+  <si>
+    <t>Bhagyasree.N</t>
+  </si>
+  <si>
+    <t>Bhargavi Bhargavi</t>
+  </si>
+  <si>
+    <t>Chaandan Banerjee</t>
+  </si>
+  <si>
+    <t>Deepak Naita</t>
+  </si>
+  <si>
+    <t>Eknath Vashishtha</t>
+  </si>
+  <si>
+    <t>Hemalatha Enugu</t>
+  </si>
+  <si>
+    <t>Hritvik Dekate</t>
+  </si>
+  <si>
+    <t>Karthika Rajaram</t>
+  </si>
+  <si>
+    <t>Kumari Divya</t>
+  </si>
+  <si>
+    <t>Manoj Pradhan</t>
+  </si>
+  <si>
+    <t>Megha R</t>
+  </si>
+  <si>
+    <t>Modugula Supriya</t>
+  </si>
+  <si>
+    <t>Nandini S</t>
+  </si>
+  <si>
+    <t>Nikhil Dhaka</t>
+  </si>
+  <si>
+    <t>Pankaj Rawat</t>
+  </si>
+  <si>
+    <t>Piyush Goyal</t>
+  </si>
+  <si>
+    <t>Sandhya Shiramagond</t>
+  </si>
+  <si>
+    <t>Sathish Kumar K</t>
+  </si>
+  <si>
+    <t>SATHISH RANGAN</t>
+  </si>
+  <si>
+    <t>Sivaraman L</t>
+  </si>
+  <si>
+    <t>Sriram Sarveswaran</t>
+  </si>
+  <si>
+    <t>Subham</t>
+  </si>
+  <si>
+    <t>Subhani Shaik</t>
+  </si>
+  <si>
+    <t>Sunil Pallath Sagar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +329,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -266,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -283,11 +372,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -298,9 +411,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,353 +732,433 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B36EF9-46CD-4CC3-AD61-091FBC495031}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.453125" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="16" thickBot="1">
+      <c r="A1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" ht="15" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A3" s="2" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1">
+      <c r="A3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A4" s="2" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A5" s="2" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1">
+      <c r="A5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A6" s="2" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1">
+      <c r="A6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A7" s="2" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1">
+      <c r="A7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A8" s="2" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A9" s="2" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A10" s="2" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1">
+      <c r="A10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A11" s="2" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1">
+      <c r="A11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A12" s="2" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1">
+      <c r="A12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A13" s="2" t="s">
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1">
+      <c r="A13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A14" s="2" t="s">
+      <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1">
+      <c r="A14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A15" s="2" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1">
+      <c r="A15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A16" s="2" t="s">
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1">
+      <c r="A16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A17" s="2" t="s">
+      <c r="F16" s="2"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1">
+      <c r="A17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A18" s="2" t="s">
+      <c r="F17" s="2"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1">
+      <c r="A18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A19" s="2" t="s">
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1">
+      <c r="A19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A20" s="2" t="s">
+      <c r="F19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1">
+      <c r="A20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A21" s="2" t="s">
+      <c r="F20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1">
+      <c r="A21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A22" s="2" t="s">
+      <c r="F21" s="2"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1">
+      <c r="A22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A23" s="2" t="s">
+      <c r="F22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1">
+      <c r="A23" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A24" s="2" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1">
+      <c r="A24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A25" s="2" t="s">
+      <c r="F24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1">
+      <c r="A25" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="2" t="s">
+      <c r="F25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="28" spans="1:7" s="4" customFormat="1">
-      <c r="A28" s="6" t="s">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="28" spans="1:8" s="4" customFormat="1">
+      <c r="A28"/>
+      <c r="B28" s="6" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>